<commit_message>
Changed Excel workbooks to fix typos
</commit_message>
<xml_diff>
--- a/files/suppliers/supplier_markers.xlsx
+++ b/files/suppliers/supplier_markers.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ollip\Documents\!!ProjectFiles\ezrab_feedbc\files\suppliers\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\viu.int.viu.ca\redirects\b\boersmao\Desktop\Presenter FIles\ezrab_feedbc\files\suppliers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2012B3B-DB90-4FE3-A31F-28A6532CB888}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1050" yWindow="1755" windowWidth="23700" windowHeight="13215" xr2:uid="{DE3B3C94-3581-4ABC-BA3E-E2502BDA4B9E}"/>
+    <workbookView xWindow="1056" yWindow="1752" windowWidth="23700" windowHeight="13212"/>
   </bookViews>
   <sheets>
     <sheet name="supplier_markers" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -536,9 +535,6 @@
     <t>Maureen Simon Foods</t>
   </si>
   <si>
-    <t>Maureen’s is a local food manufacturer in Vancouver, B.C. Canada. We create unique plant-based, local-ethnic, original food products. At Maureen’s we are based on cooking from ‘long ago’. Caribbean cooking traditionally uses a lot of veggie-focused dishes and the flavours we lean on do their best to bring out the best in veg.w</t>
-  </si>
-  <si>
     <t>19879 72nd Ave, Langley, BC</t>
   </si>
   <si>
@@ -551,9 +547,6 @@
     <t>https://maureensimonfoods.com/</t>
   </si>
   <si>
-    <t>Tofu Scramble Roll - "Rolliis"</t>
-  </si>
-  <si>
     <t>A stack of Maureens Tofu Scramble Rolliis on a wood panel backdrop.</t>
   </si>
   <si>
@@ -585,12 +578,18 @@
   </si>
   <si>
     <t>49.03713354895528, -122.27573684730973</t>
+  </si>
+  <si>
+    <t>Maureen’s is a local food manufacturer in Vancouver, B.C. Canada. We create unique plant-based, local-ethnic, original food products. At Maureen’s we are based on cooking from ‘long ago’. Caribbean cooking traditionally uses a lot of veggie-focused dishes and the flavours we lean on do their best to bring out the best in veg.</t>
+  </si>
+  <si>
+    <t>Tofu Scramble Roll - (Rolliis)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -661,7 +660,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
     </dxf>
@@ -677,7 +675,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
     </dxf>
@@ -698,17 +695,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D46F69E7-68AE-4588-AA01-B634AABE8A32}" name="Table3" displayName="Table3" ref="A1:H23" totalsRowShown="0">
-  <autoFilter ref="A1:H23" xr:uid="{D46F69E7-68AE-4588-AA01-B634AABE8A32}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:H23" totalsRowShown="0">
+  <autoFilter ref="A1:H23"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{D0D1425D-16A9-4411-96E6-CDFE62E59035}" name="Name"/>
-    <tableColumn id="2" xr3:uid="{C11F331A-B28E-405D-A1CE-45BD6ECE2CFE}" name="Address"/>
-    <tableColumn id="3" xr3:uid="{8BD2F877-E580-4FDC-9B9B-718C0C8D7B05}" name="Coordinates"/>
-    <tableColumn id="8" xr3:uid="{75CC9F10-AA28-494C-8FAC-38458856CE26}" name="Ingredients" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{B632A74E-E5AC-49E8-9360-E735C3AFF3D8}" name="Description"/>
-    <tableColumn id="5" xr3:uid="{B5554181-5001-45D9-852A-6D31E5E8C726}" name="ImageName"/>
-    <tableColumn id="6" xr3:uid="{D7FBA4B9-EA57-46D1-A1DB-F1B73391830B}" name="ImageDescription" dataDxfId="1" dataCellStyle="Hyperlink"/>
-    <tableColumn id="7" xr3:uid="{01F02F46-6D43-489F-967A-C0B014B7F3B4}" name="WebLink" dataDxfId="0" dataCellStyle="Hyperlink"/>
+    <tableColumn id="1" name="Name"/>
+    <tableColumn id="2" name="Address"/>
+    <tableColumn id="3" name="Coordinates"/>
+    <tableColumn id="8" name="Ingredients" dataDxfId="2"/>
+    <tableColumn id="4" name="Description"/>
+    <tableColumn id="5" name="ImageName"/>
+    <tableColumn id="6" name="ImageDescription" dataDxfId="1" dataCellStyle="Hyperlink"/>
+    <tableColumn id="7" name="WebLink" dataDxfId="0" dataCellStyle="Hyperlink"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1010,26 +1007,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DD1F159-8100-4025-A30A-B70436F957AB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1"/>
-    <col min="4" max="4" width="34.85546875" customWidth="1"/>
-    <col min="5" max="5" width="70.85546875" customWidth="1"/>
-    <col min="6" max="6" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="39.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" customWidth="1"/>
+    <col min="3" max="3" width="15.109375" customWidth="1"/>
+    <col min="4" max="4" width="34.88671875" customWidth="1"/>
+    <col min="5" max="5" width="70.88671875" customWidth="1"/>
+    <col min="6" max="6" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="39.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1055,7 +1052,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1081,7 +1078,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>127</v>
       </c>
@@ -1107,7 +1104,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>136</v>
       </c>
@@ -1121,7 +1118,7 @@
         <v>139</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F4" t="s">
         <v>140</v>
@@ -1133,7 +1130,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1159,7 +1156,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -1185,7 +1182,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -1211,7 +1208,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -1237,7 +1234,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>54</v>
       </c>
@@ -1263,7 +1260,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>62</v>
       </c>
@@ -1289,7 +1286,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>71</v>
       </c>
@@ -1315,7 +1312,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>79</v>
       </c>
@@ -1341,7 +1338,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>87</v>
       </c>
@@ -1367,7 +1364,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>90</v>
       </c>
@@ -1393,7 +1390,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>103</v>
       </c>
@@ -1419,7 +1416,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>111</v>
       </c>
@@ -1445,7 +1442,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>117</v>
       </c>
@@ -1471,7 +1468,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>128</v>
       </c>
@@ -1497,7 +1494,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>144</v>
       </c>
@@ -1521,7 +1518,7 @@
       </c>
       <c r="H19" s="4"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>149</v>
       </c>
@@ -1529,7 +1526,7 @@
         <v>150</v>
       </c>
       <c r="C20" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>151</v>
@@ -1547,7 +1544,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>156</v>
       </c>
@@ -1573,78 +1570,78 @@
         <v>158</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>165</v>
       </c>
       <c r="B22" t="s">
+        <v>166</v>
+      </c>
+      <c r="C22" t="s">
         <v>167</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="E22" t="s">
+        <v>181</v>
+      </c>
+      <c r="F22" t="s">
         <v>168</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="G22" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>171</v>
       </c>
-      <c r="E22" t="s">
-        <v>166</v>
-      </c>
-      <c r="F22" t="s">
-        <v>169</v>
-      </c>
-      <c r="G22" s="4" t="s">
+      <c r="B23" t="s">
+        <v>174</v>
+      </c>
+      <c r="C23" t="s">
+        <v>173</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="E23" t="s">
         <v>172</v>
       </c>
-      <c r="H22" s="2" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>173</v>
-      </c>
-      <c r="B23" t="s">
+      <c r="F23" t="s">
+        <v>175</v>
+      </c>
+      <c r="G23" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="C23" t="s">
-        <v>175</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="E23" t="s">
-        <v>174</v>
-      </c>
-      <c r="F23" t="s">
+      <c r="H23" s="2" t="s">
         <v>177</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>179</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H3" r:id="rId1" xr:uid="{7CA77C80-BAD7-4A2C-9A65-BF9E83E0AC6B}"/>
-    <hyperlink ref="H6" r:id="rId2" xr:uid="{FBF00ADD-3246-492A-956A-519785E07509}"/>
-    <hyperlink ref="H5" r:id="rId3" xr:uid="{6C4C6374-23B9-4DD0-9256-08447040F15B}"/>
-    <hyperlink ref="H2" r:id="rId4" xr:uid="{76D4D40D-5CD9-4EC2-9404-E8CE377EE168}"/>
-    <hyperlink ref="H7" r:id="rId5" xr:uid="{BF68116D-0CF0-4FC2-BD7D-53F0ACD487C3}"/>
-    <hyperlink ref="H8" r:id="rId6" xr:uid="{9722089B-356B-4FBF-89C6-D85FA9C966DA}"/>
-    <hyperlink ref="H9" r:id="rId7" xr:uid="{152DA609-651A-4517-856E-43F575774868}"/>
-    <hyperlink ref="H10" r:id="rId8" xr:uid="{C389FD6F-F7F4-4A2A-82EC-94900EF22F94}"/>
-    <hyperlink ref="H13" r:id="rId9" xr:uid="{149FDC7F-3B25-4855-B0B6-F8794EFF27DB}"/>
-    <hyperlink ref="H14" r:id="rId10" xr:uid="{719377A4-7A46-49C8-AE75-990492457310}"/>
-    <hyperlink ref="H15" r:id="rId11" xr:uid="{6315A5E9-D32E-42C5-B561-075CE885DACE}"/>
-    <hyperlink ref="H16" r:id="rId12" xr:uid="{A16A4E8D-8332-4E5A-B482-B1A94587E26C}"/>
-    <hyperlink ref="H17" r:id="rId13" xr:uid="{48EBBD19-0F00-46B0-9EA4-90C412B0247F}"/>
-    <hyperlink ref="H18" r:id="rId14" xr:uid="{770E4748-0D6A-4ECD-9194-E59E5344484F}"/>
-    <hyperlink ref="H20" r:id="rId15" xr:uid="{749B6E7F-2328-4F43-BCBD-962A46EB0F03}"/>
-    <hyperlink ref="H21" r:id="rId16" xr:uid="{FA6C07F6-AF7D-4EF6-BB9C-94D99BDA0099}"/>
-    <hyperlink ref="H22" r:id="rId17" xr:uid="{325D24F5-52CA-46A6-8DF6-C27EAC0B21C1}"/>
-    <hyperlink ref="H23" r:id="rId18" xr:uid="{496B679C-E103-4CE0-9179-17F0E02E5CCE}"/>
+    <hyperlink ref="H3" r:id="rId1"/>
+    <hyperlink ref="H6" r:id="rId2"/>
+    <hyperlink ref="H5" r:id="rId3"/>
+    <hyperlink ref="H2" r:id="rId4"/>
+    <hyperlink ref="H7" r:id="rId5"/>
+    <hyperlink ref="H8" r:id="rId6"/>
+    <hyperlink ref="H9" r:id="rId7"/>
+    <hyperlink ref="H10" r:id="rId8"/>
+    <hyperlink ref="H13" r:id="rId9"/>
+    <hyperlink ref="H14" r:id="rId10"/>
+    <hyperlink ref="H15" r:id="rId11"/>
+    <hyperlink ref="H16" r:id="rId12"/>
+    <hyperlink ref="H17" r:id="rId13"/>
+    <hyperlink ref="H18" r:id="rId14"/>
+    <hyperlink ref="H20" r:id="rId15"/>
+    <hyperlink ref="H21" r:id="rId16"/>
+    <hyperlink ref="H22" r:id="rId17"/>
+    <hyperlink ref="H23" r:id="rId18"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId19"/>

</xml_diff>